<commit_message>
Fully consumed the utilities but unable to get cell data
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="170">
   <si>
     <t>Keyword</t>
   </si>
@@ -97,30 +97,12 @@
     <t>click</t>
   </si>
   <si>
-    <t>TS_006</t>
-  </si>
-  <si>
-    <t>Wait for Some time</t>
-  </si>
-  <si>
     <t>waitFor</t>
   </si>
   <si>
-    <t>TS_007</t>
-  </si>
-  <si>
-    <t>Click on LogOut button</t>
-  </si>
-  <si>
     <t>btn_LogOut</t>
   </si>
   <si>
-    <t>TS_008</t>
-  </si>
-  <si>
-    <t>TS_009</t>
-  </si>
-  <si>
     <t>Page_Object</t>
   </si>
   <si>
@@ -130,12 +112,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Verify the text</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>verify</t>
   </si>
   <si>
@@ -145,9 +121,6 @@
     <t>Identifier</t>
   </si>
   <si>
-    <t>http://newtours.demoaut.com/</t>
-  </si>
-  <si>
     <t>Wait for a while</t>
   </si>
   <si>
@@ -181,9 +154,6 @@
     <t>evaluate</t>
   </si>
   <si>
-    <t>SIGN-OFF</t>
-  </si>
-  <si>
     <t>btn_MyAccount</t>
   </si>
   <si>
@@ -193,15 +163,9 @@
     <t>place_dropdown</t>
   </si>
   <si>
-    <t>//*[@name='userName']</t>
-  </si>
-  <si>
     <t>//*[@name='password']</t>
   </si>
   <si>
-    <t>//*[@name='login']</t>
-  </si>
-  <si>
     <t>//*[@id='account']/a</t>
   </si>
   <si>
@@ -505,12 +469,6 @@
     <t>Append query string if parameterized</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>Login to app and verify signoff text</t>
   </si>
   <si>
@@ -563,6 +521,21 @@
   </si>
   <si>
     <t>POOJA</t>
+  </si>
+  <si>
+    <t>//*[@name='email']</t>
+  </si>
+  <si>
+    <t>//*[contains(text(),'Log In')]</t>
+  </si>
+  <si>
+    <t>ccylim@unionbankph.com</t>
+  </si>
+  <si>
+    <t>P@ssw0rd123!</t>
+  </si>
+  <si>
+    <t>https://chain.unionbankph.com/i2i/home</t>
   </si>
 </sst>
 </file>
@@ -801,7 +774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -850,6 +823,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1267,13 +1243,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1284,13 +1260,13 @@
         <v>11</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1298,16 +1274,16 @@
         <v>15</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1315,349 +1291,349 @@
         <v>22</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="18" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="18" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="18" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="18" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="18" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="18" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="43.5">
       <c r="A13" s="18" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="18" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="22" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="18" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="22" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E17" s="20"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="22" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="24" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="24" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="24" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="29.25">
       <c r="A22" s="24" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="24" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="24" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1">
       <c r="A25" s="25" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="26" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1665,17 +1641,17 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1704,7 +1680,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1727,10 +1703,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -1738,90 +1714,90 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1831,11 +1807,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1860,21 +1836,21 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
@@ -1888,22 +1864,22 @@
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="11" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="5">
@@ -1912,7 +1888,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -1926,13 +1902,13 @@
       <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>159</v>
+      <c r="G4" s="28" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>16</v>
@@ -1946,13 +1922,13 @@
       <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>160</v>
+      <c r="G5" s="28" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>19</v>
@@ -1969,95 +1945,21 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="3" t="s">
-        <v>173</v>
-      </c>
+      <c r="G7" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2066,7 +1968,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2077,10 +1979,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2088,7 +1990,7 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2096,7 +1998,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2104,199 +2006,199 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="8" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="8" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="8" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="8" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="8" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="8" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="8" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2324,7 +2226,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2332,10 +2234,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2343,13 +2245,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2374,51 +2276,51 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C1" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>